<commit_message>
update relation of person
</commit_message>
<xml_diff>
--- a/static/templates/excel/人员导入模板.xlsx
+++ b/static/templates/excel/人员导入模板.xlsx
@@ -21,11 +21,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t xml:space="preserve">姓名</t>
   </si>
   <si>
+    <t xml:space="preserve">与其他人员关系</t>
+  </si>
+  <si>
     <t xml:space="preserve">身份证号</t>
   </si>
   <si>
@@ -108,6 +111,9 @@
   </si>
   <si>
     <t xml:space="preserve">必填，真实姓名</t>
+  </si>
+  <si>
+    <t xml:space="preserve">如：户主、配偶、子女、父母、租户（可选）</t>
   </si>
   <si>
     <t xml:space="preserve">必填，18位身份证号</t>
@@ -196,7 +202,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +233,13 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -270,7 +283,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -279,16 +292,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -483,41 +504,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB1048576"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:AB1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,7 +548,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -605,95 +626,99 @@
       <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="L2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="V2" s="4" t="s">
+      <c r="P2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="R2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="U2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="X2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Y2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="Z2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AA2" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="AB2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -713,7 +738,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="A1:AB1 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -722,23 +747,23 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>51</v>
+      <c r="A1" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>52</v>
+      <c r="A2" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>53</v>
+      <c r="A3" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>